<commit_message>
Changes for NIME, mostly just sorting out the spreadsheet examples
</commit_message>
<xml_diff>
--- a/Excel Music.xlsx
+++ b/Excel Music.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21402"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{234A0567-2A56-4259-AA57-FB42CBB9EE5E}" xr6:coauthVersionLast="42" xr6:coauthVersionMax="42" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="28125"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-680" yWindow="0" windowWidth="25360" windowHeight="14220"/>
   </bookViews>
   <sheets>
     <sheet name="Tutorial" sheetId="6" r:id="rId1"/>
@@ -16,8 +15,11 @@
     <sheet name="Exercise 2 Solution" sheetId="10" state="hidden" r:id="rId6"/>
     <sheet name="Christmas" sheetId="5" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
@@ -28,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1352" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1350" uniqueCount="234">
   <si>
     <t>Welcome to my music in Excel prototype 📊🎵. Here's how it works!</t>
   </si>
@@ -705,21 +707,6 @@
     <t>Right Hand</t>
   </si>
   <si>
-    <t>!turtle(B13, EL13, 1, 1)</t>
-  </si>
-  <si>
-    <t>!turtle(B8:B11, r m142, 1,1)</t>
-  </si>
-  <si>
-    <t>!turtle(B14,r m142, 1, 1)</t>
-  </si>
-  <si>
-    <t>!turtle(B15:B16,r m142, 1, 1)</t>
-  </si>
-  <si>
-    <t>s,G5</t>
-  </si>
-  <si>
     <t>G5</t>
   </si>
   <si>
@@ -736,13 +723,22 @@
   </si>
   <si>
     <t>G2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -,G5</t>
+  </si>
+  <si>
+    <t>!turtle(B13:B16, rm*, 1, 1)</t>
+  </si>
+  <si>
+    <t>!turtle(B8:B11, r m*, 1,1)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -793,6 +789,14 @@
       <b/>
       <sz val="14"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -937,9 +941,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -993,7 +998,8 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -1053,7 +1059,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1105,7 +1111,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1299,21 +1305,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6F03C6F-C8D8-494B-AFC6-46ACA29E7514}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L108"/>
   <sheetViews>
-    <sheetView topLeftCell="A53" workbookViewId="0" xr3:uid="{B78AD311-3778-5721-86A4-8184A4FC7F89}">
-      <selection activeCell="A67" sqref="A67"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:12" ht="16.5" customHeight="1">
       <c r="A1" s="1" t="s">
@@ -3203,31 +3209,36 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{130CC00D-DDCD-477C-9E1B-77F36A08060B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z47"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" workbookViewId="0" xr3:uid="{9017BC1D-BD7F-5FED-AF86-FB279A6496C3}">
+    <sheetView topLeftCell="A17" workbookViewId="0">
       <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="8" customWidth="1"/>
-    <col min="2" max="2" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="18" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="4.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="18" width="5.1640625" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="4" bestFit="1" customWidth="1"/>
-    <col min="20" max="25" width="3.7109375" customWidth="1"/>
+    <col min="20" max="25" width="3.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="18.75">
+    <row r="1" spans="1:24" ht="18">
       <c r="A1" s="38" t="s">
         <v>141</v>
       </c>
@@ -4903,25 +4914,30 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{672125CA-7AD2-4368-9BC9-51753DC4E351}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AW19"/>
   <sheetViews>
-    <sheetView workbookViewId="0" xr3:uid="{4BE764D4-38B5-570C-B973-31E03DE099C0}">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="25.42578125" customWidth="1"/>
-    <col min="2" max="2" width="4.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.5" customWidth="1"/>
+    <col min="2" max="2" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.5" bestFit="1" customWidth="1"/>
     <col min="4" max="6" width="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="18" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="22" width="4.42578125" customWidth="1"/>
+    <col min="7" max="18" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="22" width="4.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:49">
@@ -5303,32 +5319,36 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A3" r:id="rId1" xr:uid="{A2244A1C-32D2-48A9-8879-0C20251EBEB1}"/>
+    <hyperlink ref="A3" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15585C32-A4C4-4C66-9C93-C0B2BAC5B884}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AW10"/>
   <sheetViews>
-    <sheetView workbookViewId="0" xr3:uid="{2A73514B-63D7-5113-A6A0-B81A19636E81}">
+    <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13:J14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="6" width="3.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="4.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="6" width="3.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="3.5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="3.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="4.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="12" width="4.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="4.5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="3.5" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5806,54 +5826,59 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{FF766697-1CB6-4BCB-A586-2A0A9C37FD6B}"/>
+    <hyperlink ref="A2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35E7C1DB-29FE-4B83-8804-C2A766460DAF}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG15"/>
   <sheetViews>
-    <sheetView workbookViewId="0" xr3:uid="{BA2D3206-DD76-55E9-B797-7C6577EED279}">
+    <sheetView workbookViewId="0">
       <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="3.140625" customWidth="1"/>
-    <col min="4" max="4" width="4.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="2.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="4.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="2.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.1640625" customWidth="1"/>
+    <col min="4" max="4" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="2.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="2.5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="4.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="3.5" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="4.5" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="2" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="5" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="2.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="4.140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="3.140625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="4.140625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="2.5703125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="4.140625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="2.5703125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="4.28515625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="2.5" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="2.5" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="4.5" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="4.5" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="2.5" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="4.5" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="3.5" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="2" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="4.5" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="2" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="5" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="3.140625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="3.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:33">
@@ -6389,33 +6414,38 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D74FA5F-3809-4670-AC21-9FF2E1BC79D4}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q15"/>
   <sheetViews>
-    <sheetView workbookViewId="0" xr3:uid="{8776BC61-746F-5351-9007-E328B7949851}">
+    <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="3.140625" customWidth="1"/>
-    <col min="4" max="4" width="3.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="2.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.1640625" customWidth="1"/>
+    <col min="4" max="4" width="3.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="2.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="3.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="2.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="2.5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="6" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="4.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="4.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="5.6640625" bestFit="1" customWidth="1"/>
     <col min="15" max="16" width="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="2.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="2.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
@@ -6911,144 +6941,148 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A12DF2A-C80B-43FB-8B54-676DDFD39A82}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:EL19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0" xr3:uid="{1A6C6700-72C2-5D87-85B4-28624D5879F1}">
-      <selection activeCell="A20" sqref="A20:XFD29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.28515625" customWidth="1"/>
-    <col min="4" max="4" width="4.7109375" customWidth="1"/>
-    <col min="5" max="5" width="4.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="3.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="4.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="3.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="4.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="3.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="3.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="4.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="4.140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="3.42578125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="3.140625" bestFit="1" customWidth="1"/>
-    <col min="20" max="21" width="3.42578125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="3.140625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="4.33203125" customWidth="1"/>
+    <col min="4" max="4" width="4.6640625" customWidth="1"/>
+    <col min="5" max="5" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="3.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="3.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="4.83203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="4.5" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="3.5" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="21" width="3.5" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="3.5" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="2" bestFit="1" customWidth="1"/>
-    <col min="25" max="26" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="25" max="26" width="3.5" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="2" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="3.42578125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="3.5" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="4.33203125" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="2" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="3.42578125" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="4.28515625" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="3.42578125" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="3.28515625" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="3.5" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="3.5" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="3.33203125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="4.33203125" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="2" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="3.42578125" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="3.5" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="4.33203125" bestFit="1" customWidth="1"/>
     <col min="39" max="39" width="2" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="3.42578125" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="4.28515625" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="4.140625" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="3.42578125" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="3.5" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="3.5" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="4.1640625" bestFit="1" customWidth="1"/>
     <col min="45" max="45" width="2" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="3.28515625" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="3.42578125" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="4.28515625" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="3.33203125" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="3.5" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="4.5" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="3.5" bestFit="1" customWidth="1"/>
     <col min="51" max="51" width="2" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="3.28515625" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="3.33203125" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="4.33203125" bestFit="1" customWidth="1"/>
     <col min="54" max="54" width="2" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="3.42578125" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="3.5" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="4.5" bestFit="1" customWidth="1"/>
     <col min="57" max="58" width="2" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="4.28515625" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="3.28515625" bestFit="1" customWidth="1"/>
-    <col min="61" max="62" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="3.33203125" bestFit="1" customWidth="1"/>
+    <col min="61" max="62" width="3.5" bestFit="1" customWidth="1"/>
     <col min="63" max="63" width="2" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="3.140625" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="4.140625" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="3.140625" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="3.1640625" bestFit="1" customWidth="1"/>
     <col min="67" max="67" width="2" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="3.5" bestFit="1" customWidth="1"/>
     <col min="69" max="69" width="2" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="3.140625" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="4.140625" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="3.42578125" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="4.140625" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="3.5" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="3.5" bestFit="1" customWidth="1"/>
     <col min="75" max="75" width="2" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="3.28515625" bestFit="1" customWidth="1"/>
-    <col min="77" max="77" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="3.33203125" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="3.5" bestFit="1" customWidth="1"/>
     <col min="78" max="78" width="2" bestFit="1" customWidth="1"/>
-    <col min="79" max="79" width="3.42578125" bestFit="1" customWidth="1"/>
-    <col min="80" max="80" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="3.5" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="4.33203125" bestFit="1" customWidth="1"/>
     <col min="81" max="82" width="2" bestFit="1" customWidth="1"/>
-    <col min="83" max="83" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="4.33203125" bestFit="1" customWidth="1"/>
     <col min="84" max="84" width="2" bestFit="1" customWidth="1"/>
-    <col min="85" max="86" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="85" max="86" width="3.5" bestFit="1" customWidth="1"/>
     <col min="87" max="87" width="2" bestFit="1" customWidth="1"/>
-    <col min="88" max="88" width="3.140625" bestFit="1" customWidth="1"/>
-    <col min="89" max="89" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="88" max="88" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="89" max="89" width="4.33203125" bestFit="1" customWidth="1"/>
     <col min="90" max="90" width="2" bestFit="1" customWidth="1"/>
-    <col min="91" max="91" width="3.140625" bestFit="1" customWidth="1"/>
-    <col min="92" max="92" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="91" max="91" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="92" max="92" width="4.1640625" bestFit="1" customWidth="1"/>
     <col min="93" max="93" width="2" bestFit="1" customWidth="1"/>
-    <col min="94" max="94" width="3.140625" bestFit="1" customWidth="1"/>
-    <col min="95" max="95" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="94" max="94" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="95" max="95" width="4.1640625" bestFit="1" customWidth="1"/>
     <col min="96" max="97" width="2" bestFit="1" customWidth="1"/>
-    <col min="98" max="98" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="98" max="98" width="3.5" bestFit="1" customWidth="1"/>
     <col min="99" max="99" width="2" bestFit="1" customWidth="1"/>
-    <col min="100" max="100" width="3.28515625" bestFit="1" customWidth="1"/>
-    <col min="101" max="101" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="100" max="100" width="3.33203125" bestFit="1" customWidth="1"/>
+    <col min="101" max="101" width="4.33203125" bestFit="1" customWidth="1"/>
     <col min="102" max="102" width="2" bestFit="1" customWidth="1"/>
-    <col min="103" max="103" width="4.28515625" bestFit="1" customWidth="1"/>
-    <col min="104" max="104" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="103" max="103" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="104" max="104" width="4.1640625" bestFit="1" customWidth="1"/>
     <col min="105" max="106" width="2" bestFit="1" customWidth="1"/>
-    <col min="107" max="107" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="107" max="107" width="4.33203125" bestFit="1" customWidth="1"/>
     <col min="108" max="109" width="2" bestFit="1" customWidth="1"/>
-    <col min="110" max="110" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="110" max="110" width="4.1640625" bestFit="1" customWidth="1"/>
     <col min="111" max="111" width="2" bestFit="1" customWidth="1"/>
-    <col min="112" max="112" width="4.140625" bestFit="1" customWidth="1"/>
-    <col min="113" max="113" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="112" max="112" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="113" max="113" width="3.5" bestFit="1" customWidth="1"/>
     <col min="114" max="114" width="2" bestFit="1" customWidth="1"/>
-    <col min="115" max="115" width="3.140625" bestFit="1" customWidth="1"/>
-    <col min="116" max="116" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="115" max="115" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="116" max="116" width="3.5" bestFit="1" customWidth="1"/>
     <col min="117" max="118" width="2" bestFit="1" customWidth="1"/>
-    <col min="119" max="119" width="3.140625" bestFit="1" customWidth="1"/>
+    <col min="119" max="119" width="3.1640625" bestFit="1" customWidth="1"/>
     <col min="120" max="121" width="2" bestFit="1" customWidth="1"/>
-    <col min="122" max="123" width="3.42578125" bestFit="1" customWidth="1"/>
-    <col min="124" max="124" width="3.28515625" bestFit="1" customWidth="1"/>
-    <col min="125" max="125" width="4.28515625" bestFit="1" customWidth="1"/>
-    <col min="126" max="126" width="3.28515625" bestFit="1" customWidth="1"/>
-    <col min="127" max="127" width="4.28515625" bestFit="1" customWidth="1"/>
-    <col min="128" max="128" width="4.140625" bestFit="1" customWidth="1"/>
-    <col min="129" max="130" width="3.42578125" bestFit="1" customWidth="1"/>
-    <col min="131" max="131" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="122" max="123" width="3.5" bestFit="1" customWidth="1"/>
+    <col min="124" max="124" width="3.33203125" bestFit="1" customWidth="1"/>
+    <col min="125" max="125" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="126" max="126" width="3.33203125" bestFit="1" customWidth="1"/>
+    <col min="127" max="127" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="128" max="128" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="129" max="130" width="3.5" bestFit="1" customWidth="1"/>
+    <col min="131" max="131" width="4.33203125" bestFit="1" customWidth="1"/>
     <col min="132" max="132" width="2" bestFit="1" customWidth="1"/>
-    <col min="133" max="133" width="3.42578125" bestFit="1" customWidth="1"/>
-    <col min="134" max="134" width="4.140625" bestFit="1" customWidth="1"/>
-    <col min="135" max="135" width="3.42578125" bestFit="1" customWidth="1"/>
-    <col min="136" max="136" width="4.140625" bestFit="1" customWidth="1"/>
-    <col min="137" max="137" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="138" max="138" width="3.42578125" bestFit="1" customWidth="1"/>
-    <col min="139" max="139" width="3.140625" bestFit="1" customWidth="1"/>
-    <col min="140" max="140" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="133" max="133" width="3.5" bestFit="1" customWidth="1"/>
+    <col min="134" max="134" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="135" max="135" width="3.5" bestFit="1" customWidth="1"/>
+    <col min="136" max="136" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="137" max="137" width="4.5" bestFit="1" customWidth="1"/>
+    <col min="138" max="138" width="3.5" bestFit="1" customWidth="1"/>
+    <col min="139" max="139" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="140" max="140" width="3.5" bestFit="1" customWidth="1"/>
     <col min="141" max="142" width="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -7342,20 +7376,19 @@
       <c r="EK2" s="1"/>
       <c r="EL2" s="1"/>
     </row>
-    <row r="3" spans="1:142" ht="15.75">
+    <row r="3" spans="1:142" ht="15">
       <c r="A3" s="1"/>
       <c r="B3" s="28" t="s">
         <v>223</v>
       </c>
       <c r="C3" s="1"/>
-      <c r="D3" s="28" t="s">
-        <v>224</v>
-      </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
+      <c r="I3" s="28" t="s">
+        <v>224</v>
+      </c>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
@@ -7493,17 +7526,16 @@
     <row r="4" spans="1:142">
       <c r="A4" s="1"/>
       <c r="B4" s="3" t="s">
-        <v>225</v>
+        <v>232</v>
       </c>
       <c r="C4" s="1"/>
-      <c r="D4" s="3" t="s">
-        <v>226</v>
-      </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
+      <c r="I4" s="3" t="s">
+        <v>233</v>
+      </c>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
@@ -7640,9 +7672,6 @@
     </row>
     <row r="5" spans="1:142">
       <c r="A5" s="1"/>
-      <c r="B5" s="3" t="s">
-        <v>227</v>
-      </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -7786,9 +7815,6 @@
     </row>
     <row r="6" spans="1:142">
       <c r="A6" s="1"/>
-      <c r="B6" s="3" t="s">
-        <v>228</v>
-      </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -8186,7 +8212,7 @@
         <v>199</v>
       </c>
       <c r="O8" s="9" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="P8" s="9" t="s">
         <v>199</v>
@@ -8287,10 +8313,10 @@
         <v>201</v>
       </c>
       <c r="DD8" s="22" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="DE8" s="22" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="DF8" s="8"/>
       <c r="DG8" s="8"/>
@@ -8320,7 +8346,7 @@
         <v>199</v>
       </c>
       <c r="EE8" s="9" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="EF8" s="9" t="s">
         <v>199</v>
@@ -8347,19 +8373,19 @@
         <v>201</v>
       </c>
       <c r="L9" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="M9" s="13" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="N9" s="13" t="s">
         <v>77</v>
       </c>
       <c r="O9" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="P9" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="Q9" s="13" t="s">
         <v>125</v>
@@ -8387,7 +8413,7 @@
         <v>201</v>
       </c>
       <c r="AJ9" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="AK9" s="13" t="s">
         <v>201</v>
@@ -8399,55 +8425,55 @@
         <v>199</v>
       </c>
       <c r="AP9" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="AQ9" s="13" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="AR9" s="13" t="s">
         <v>201</v>
       </c>
       <c r="AS9" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="AT9" s="13" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="AU9" s="13" t="s">
         <v>201</v>
       </c>
       <c r="AV9" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="AW9" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="AX9" s="13" t="s">
         <v>201</v>
       </c>
       <c r="AY9" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="AZ9" s="13" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="BA9" s="13" t="s">
         <v>201</v>
       </c>
       <c r="BB9" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="BC9" s="13" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="BD9" s="13" t="s">
         <v>73</v>
       </c>
       <c r="BE9" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="BF9" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="BG9" s="12"/>
       <c r="BH9" s="12"/>
@@ -8456,7 +8482,7 @@
         <v>125</v>
       </c>
       <c r="BK9" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="BL9" s="13" t="s">
         <v>125</v>
@@ -8468,7 +8494,7 @@
         <v>125</v>
       </c>
       <c r="BO9" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="BP9" s="12"/>
       <c r="BQ9" s="12"/>
@@ -8480,28 +8506,28 @@
         <v>201</v>
       </c>
       <c r="BW9" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="BX9" s="13" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="BY9" s="13" t="s">
         <v>201</v>
       </c>
       <c r="BZ9" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="CA9" s="13" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="CB9" s="13" t="s">
         <v>199</v>
       </c>
       <c r="CC9" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="CD9" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="CE9" s="12"/>
       <c r="CF9" s="12"/>
@@ -8510,7 +8536,7 @@
         <v>125</v>
       </c>
       <c r="CI9" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="CJ9" s="13" t="s">
         <v>125</v>
@@ -8519,7 +8545,7 @@
         <v>199</v>
       </c>
       <c r="CL9" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="CM9" s="13" t="s">
         <v>125</v>
@@ -8531,10 +8557,10 @@
         <v>199</v>
       </c>
       <c r="CR9" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="CS9" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="CT9" s="12"/>
       <c r="CU9" s="12"/>
@@ -8549,16 +8575,16 @@
         <v>125</v>
       </c>
       <c r="DD9" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="DE9" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="DF9" s="13" t="s">
         <v>199</v>
       </c>
       <c r="DG9" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="DH9" s="13" t="s">
         <v>199</v>
@@ -8567,7 +8593,7 @@
         <v>125</v>
       </c>
       <c r="DJ9" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="DK9" s="13" t="s">
         <v>125</v>
@@ -8591,19 +8617,19 @@
         <v>201</v>
       </c>
       <c r="EB9" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="EC9" s="13" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="ED9" s="13" t="s">
         <v>77</v>
       </c>
       <c r="EE9" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="EF9" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="EG9" s="13" t="s">
         <v>125</v>
@@ -8632,7 +8658,7 @@
         <v>77</v>
       </c>
       <c r="I10" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="J10" s="13" t="s">
         <v>77</v>
@@ -8641,19 +8667,19 @@
         <v>125</v>
       </c>
       <c r="L10" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="M10" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="N10" s="13" t="s">
         <v>75</v>
       </c>
       <c r="O10" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="P10" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="Q10" s="13" t="s">
         <v>77</v>
@@ -8678,7 +8704,7 @@
         <v>77</v>
       </c>
       <c r="AA10" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="AB10" s="13" t="s">
         <v>77</v>
@@ -8687,34 +8713,34 @@
         <v>199</v>
       </c>
       <c r="AD10" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="AE10" s="13" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="AF10" s="13" t="s">
         <v>201</v>
       </c>
       <c r="AG10" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="AH10" s="13" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="AI10" s="13" t="s">
         <v>125</v>
       </c>
       <c r="AJ10" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="AK10" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="AL10" s="13" t="s">
         <v>77</v>
       </c>
       <c r="AM10" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="AN10" s="13" t="s">
         <v>77</v>
@@ -8723,61 +8749,61 @@
         <v>76</v>
       </c>
       <c r="AP10" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="AQ10" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="AR10" s="13" t="s">
         <v>125</v>
       </c>
       <c r="AS10" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="AT10" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="AU10" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="AV10" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="AW10" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="AX10" s="13" t="s">
         <v>125</v>
       </c>
       <c r="AY10" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="AZ10" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="BA10" s="13" t="s">
         <v>125</v>
       </c>
       <c r="BB10" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="BC10" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="BD10" s="13" t="s">
         <v>76</v>
       </c>
       <c r="BE10" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="BF10" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="BG10" s="13" t="s">
         <v>77</v>
       </c>
       <c r="BH10" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="BI10" s="13" t="s">
         <v>77</v>
@@ -8786,17 +8812,17 @@
         <v>77</v>
       </c>
       <c r="BK10" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="BL10" s="12"/>
       <c r="BM10" s="13" t="s">
         <v>77</v>
       </c>
       <c r="BN10" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="BO10" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="BP10" s="12"/>
       <c r="BQ10" s="12"/>
@@ -8808,34 +8834,34 @@
         <v>77</v>
       </c>
       <c r="BW10" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="BX10" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="BY10" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="BZ10" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="CA10" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="CB10" s="13" t="s">
         <v>76</v>
       </c>
       <c r="CC10" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="CD10" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="CE10" s="13" t="s">
         <v>77</v>
       </c>
       <c r="CF10" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="CG10" s="13" t="s">
         <v>77</v>
@@ -8844,25 +8870,25 @@
         <v>77</v>
       </c>
       <c r="CI10" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="CJ10" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="CK10" s="13" t="s">
         <v>76</v>
       </c>
       <c r="CL10" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="CM10" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="CN10" s="13" t="s">
         <v>77</v>
       </c>
       <c r="CO10" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="CP10" s="13" t="s">
         <v>125</v>
@@ -8871,16 +8897,16 @@
         <v>77</v>
       </c>
       <c r="CR10" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="CS10" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="CT10" s="13" t="s">
         <v>75</v>
       </c>
       <c r="CU10" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="CV10" s="13" t="s">
         <v>75</v>
@@ -8889,7 +8915,7 @@
         <v>76</v>
       </c>
       <c r="CX10" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="CY10" s="13" t="s">
         <v>76</v>
@@ -8898,37 +8924,37 @@
         <v>77</v>
       </c>
       <c r="DA10" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="DB10" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="DC10" s="13" t="s">
         <v>76</v>
       </c>
       <c r="DD10" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="DE10" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="DF10" s="13" t="s">
         <v>77</v>
       </c>
       <c r="DG10" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="DH10" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="DI10" s="13" t="s">
         <v>77</v>
       </c>
       <c r="DJ10" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="DK10" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="DL10" s="12"/>
       <c r="DM10" s="12"/>
@@ -8952,7 +8978,7 @@
         <v>77</v>
       </c>
       <c r="DY10" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="DZ10" s="13" t="s">
         <v>77</v>
@@ -8961,19 +8987,19 @@
         <v>125</v>
       </c>
       <c r="EB10" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="EC10" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="ED10" s="13" t="s">
         <v>75</v>
       </c>
       <c r="EE10" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="EF10" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="EG10" s="13" t="s">
         <v>77</v>
@@ -9003,10 +9029,10 @@
         <v>74</v>
       </c>
       <c r="F11" s="24" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="G11" s="24" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="H11" s="16" t="s">
         <v>74</v>
@@ -9015,65 +9041,65 @@
         <v>74</v>
       </c>
       <c r="J11" s="24" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="K11" s="16" t="s">
         <v>76</v>
       </c>
       <c r="L11" s="24" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="M11" s="24" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="N11" s="16" t="s">
         <v>74</v>
       </c>
       <c r="O11" s="24" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="P11" s="24" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="Q11" s="16" t="s">
         <v>146</v>
       </c>
       <c r="R11" s="24" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="S11" s="24" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="T11" s="16" t="s">
         <v>75</v>
       </c>
       <c r="U11" s="24" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="V11" s="24" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="W11" s="24" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="X11" s="24" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="Y11" s="17"/>
       <c r="Z11" s="16" t="s">
         <v>160</v>
       </c>
       <c r="AA11" s="24" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="AB11" s="24" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="AC11" s="16" t="s">
         <v>76</v>
       </c>
       <c r="AD11" s="24" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="AE11" s="16" t="s">
         <v>75</v>
@@ -9085,79 +9111,79 @@
         <v>77</v>
       </c>
       <c r="AH11" s="24" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="AI11" s="16" t="s">
         <v>76</v>
       </c>
       <c r="AJ11" s="24" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="AK11" s="24" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="AL11" s="16" t="s">
         <v>76</v>
       </c>
       <c r="AM11" s="24" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="AN11" s="24" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="AO11" s="16" t="s">
         <v>74</v>
       </c>
       <c r="AP11" s="24" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="AQ11" s="24" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="AR11" s="16" t="s">
         <v>75</v>
       </c>
       <c r="AS11" s="24" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="AT11" s="24" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="AU11" s="24" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="AV11" s="24" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="AW11" s="24" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="AX11" s="16" t="s">
         <v>75</v>
       </c>
       <c r="AY11" s="24" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="AZ11" s="24" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="BA11" s="16" t="s">
         <v>76</v>
       </c>
       <c r="BB11" s="24" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="BC11" s="24" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="BD11" s="16" t="s">
         <v>205</v>
       </c>
       <c r="BE11" s="24" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="BF11" s="24" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="BG11" s="16" t="s">
         <v>76</v>
@@ -9172,23 +9198,23 @@
         <v>74</v>
       </c>
       <c r="BK11" s="24" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="BL11" s="17"/>
       <c r="BM11" s="16" t="s">
         <v>75</v>
       </c>
       <c r="BN11" s="24" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="BO11" s="24" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="BP11" s="16" t="s">
         <v>77</v>
       </c>
       <c r="BQ11" s="24" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="BR11" s="16" t="s">
         <v>125</v>
@@ -9197,7 +9223,7 @@
         <v>199</v>
       </c>
       <c r="BT11" s="24" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="BU11" s="16" t="s">
         <v>199</v>
@@ -9206,88 +9232,88 @@
         <v>74</v>
       </c>
       <c r="BW11" s="24" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="BX11" s="24" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="BY11" s="24" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="BZ11" s="24" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="CA11" s="24" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="CB11" s="16" t="s">
         <v>74</v>
       </c>
       <c r="CC11" s="24" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="CD11" s="24" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="CE11" s="16" t="s">
         <v>74</v>
       </c>
       <c r="CF11" s="24" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="CG11" s="24" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="CH11" s="16" t="s">
         <v>75</v>
       </c>
       <c r="CI11" s="24" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="CJ11" s="24" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="CK11" s="16" t="s">
         <v>74</v>
       </c>
       <c r="CL11" s="24" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="CM11" s="24" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="CN11" s="16" t="s">
         <v>74</v>
       </c>
       <c r="CO11" s="24" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="CP11" s="24" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="CQ11" s="16" t="s">
         <v>74</v>
       </c>
       <c r="CR11" s="24" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="CS11" s="24" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="CT11" s="16" t="s">
         <v>74</v>
       </c>
       <c r="CU11" s="24" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="CV11" s="24" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="CW11" s="16" t="s">
         <v>74</v>
       </c>
       <c r="CX11" s="24" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="CY11" s="16" t="s">
         <v>74</v>
@@ -9296,55 +9322,55 @@
         <v>74</v>
       </c>
       <c r="DA11" s="24" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="DB11" s="24" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="DC11" s="16" t="s">
         <v>75</v>
       </c>
       <c r="DD11" s="24" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="DE11" s="24" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="DF11" s="16" t="s">
         <v>75</v>
       </c>
       <c r="DG11" s="24" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="DH11" s="24" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="DI11" s="16" t="s">
         <v>74</v>
       </c>
       <c r="DJ11" s="24" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="DK11" s="24" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="DL11" s="16" t="s">
         <v>77</v>
       </c>
       <c r="DM11" s="24" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="DN11" s="24" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="DO11" s="24" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="DP11" s="24" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="DQ11" s="24" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="DR11" s="16" t="s">
         <v>75</v>
@@ -9359,10 +9385,10 @@
         <v>74</v>
       </c>
       <c r="DV11" s="24" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="DW11" s="24" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="DX11" s="16" t="s">
         <v>74</v>
@@ -9371,43 +9397,43 @@
         <v>74</v>
       </c>
       <c r="DZ11" s="24" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="EA11" s="16" t="s">
         <v>76</v>
       </c>
       <c r="EB11" s="24" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="EC11" s="24" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="ED11" s="16" t="s">
         <v>74</v>
       </c>
       <c r="EE11" s="24" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="EF11" s="24" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="EG11" s="16" t="s">
         <v>146</v>
       </c>
       <c r="EH11" s="24" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="EI11" s="24" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="EJ11" s="16" t="s">
         <v>77</v>
       </c>
       <c r="EK11" s="24" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="EL11" s="25" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:142">
@@ -9560,46 +9586,46 @@
         <v>91</v>
       </c>
       <c r="C13" s="22" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="D13" s="22" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="E13" s="9" t="s">
         <v>91</v>
       </c>
       <c r="F13" s="22" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="G13" s="22" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="H13" s="9" t="s">
         <v>194</v>
       </c>
       <c r="I13" s="22" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="J13" s="22" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="K13" s="9" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="L13" s="22" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="M13" s="22" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="N13" s="9" t="s">
         <v>159</v>
       </c>
       <c r="O13" s="22" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="P13" s="22" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="Q13" s="8"/>
       <c r="R13" s="8"/>
@@ -9617,25 +9643,25 @@
         <v>74</v>
       </c>
       <c r="X13" s="22" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="Y13" s="22" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="Z13" s="9" t="s">
         <v>67</v>
       </c>
       <c r="AA13" s="22" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="AB13" s="22" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="AC13" s="22" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="AD13" s="22" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="AE13" s="9" t="s">
         <v>67</v>
@@ -9644,52 +9670,52 @@
         <v>73</v>
       </c>
       <c r="AG13" s="22" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="AH13" s="22" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="AI13" s="22" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="AJ13" s="22" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="AK13" s="22" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="AL13" s="9" t="s">
         <v>73</v>
       </c>
       <c r="AM13" s="22" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="AN13" s="22" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="AO13" s="22" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="AP13" s="9" t="s">
         <v>73</v>
       </c>
       <c r="AQ13" s="22" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="AR13" s="9" t="s">
         <v>73</v>
       </c>
       <c r="AS13" s="22" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="AT13" s="22" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="AU13" s="22" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="AV13" s="9" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="AW13" s="9" t="s">
         <v>205</v>
@@ -9698,64 +9724,64 @@
         <v>74</v>
       </c>
       <c r="AY13" s="22" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="AZ13" s="22" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="BA13" s="9" t="s">
         <v>75</v>
       </c>
       <c r="BB13" s="22" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="BC13" s="22" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="BD13" s="9" t="s">
         <v>73</v>
       </c>
       <c r="BE13" s="22" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="BF13" s="22" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="BG13" s="9" t="s">
         <v>73</v>
       </c>
       <c r="BH13" s="22" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="BI13" s="22" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="BJ13" s="9" t="s">
         <v>62</v>
       </c>
       <c r="BK13" s="22" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="BL13" s="22" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="BM13" s="9" t="s">
         <v>62</v>
       </c>
       <c r="BN13" s="22" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="BO13" s="22" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="BP13" s="9" t="s">
         <v>74</v>
       </c>
       <c r="BQ13" s="22" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="BR13" s="22" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="BS13" s="8"/>
       <c r="BT13" s="8"/>
@@ -9806,64 +9832,64 @@
         <v>74</v>
       </c>
       <c r="DM13" s="22" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="DN13" s="22" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="DO13" s="22" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="DP13" s="22" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="DQ13" s="22" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="DR13" s="9" t="s">
         <v>62</v>
       </c>
       <c r="DS13" s="22" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="DT13" s="22" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="DU13" s="9" t="s">
         <v>62</v>
       </c>
       <c r="DV13" s="22" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="DW13" s="22" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="DX13" s="9" t="s">
         <v>73</v>
       </c>
       <c r="DY13" s="22" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="DZ13" s="22" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="EA13" s="9" t="s">
         <v>73</v>
       </c>
       <c r="EB13" s="22" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="EC13" s="22" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="ED13" s="9" t="s">
         <v>67</v>
       </c>
       <c r="EE13" s="22" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="EF13" s="22" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="EG13" s="8"/>
       <c r="EH13" s="8"/>
@@ -9872,22 +9898,22 @@
         <v>74</v>
       </c>
       <c r="EK13" s="22" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="EL13" s="26" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:142">
       <c r="A14" s="1"/>
       <c r="B14" s="20" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="C14" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="D14" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="E14" s="12"/>
       <c r="F14" s="12"/>
@@ -9914,16 +9940,16 @@
         <v>16</v>
       </c>
       <c r="AA14" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="AB14" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="AC14" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="AD14" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="AE14" s="13" t="s">
         <v>16</v>
@@ -9932,118 +9958,118 @@
         <v>16</v>
       </c>
       <c r="AG14" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="AH14" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="AI14" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="AJ14" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="AK14" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="AL14" s="13" t="s">
         <v>173</v>
       </c>
       <c r="AM14" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="AN14" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="AO14" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="AP14" s="13" t="s">
         <v>173</v>
       </c>
       <c r="AQ14" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="AR14" s="13" t="s">
         <v>194</v>
       </c>
       <c r="AS14" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="AT14" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="AU14" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="AV14" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="AW14" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="AX14" s="13" t="s">
         <v>16</v>
       </c>
       <c r="AY14" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="AZ14" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="BA14" s="13" t="s">
         <v>67</v>
       </c>
       <c r="BB14" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="BC14" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="BD14" s="13" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="BE14" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="BF14" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="BG14" s="13" t="s">
         <v>173</v>
       </c>
       <c r="BH14" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="BI14" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="BJ14" s="13" t="s">
         <v>7</v>
       </c>
       <c r="BK14" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="BL14" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="BM14" s="13" t="s">
         <v>160</v>
       </c>
       <c r="BN14" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="BO14" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="BP14" s="13" t="s">
         <v>67</v>
       </c>
       <c r="BQ14" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="BR14" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="BS14" s="12"/>
       <c r="BT14" s="12"/>
@@ -10052,73 +10078,73 @@
         <v>62</v>
       </c>
       <c r="BW14" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="BX14" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="BY14" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="BZ14" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="CA14" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="CB14" s="13" t="s">
         <v>67</v>
       </c>
       <c r="CC14" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="CD14" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="CE14" s="13" t="s">
         <v>76</v>
       </c>
       <c r="CF14" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="CG14" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="CH14" s="13" t="s">
         <v>62</v>
       </c>
       <c r="CI14" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="CJ14" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="CK14" s="13" t="s">
         <v>62</v>
       </c>
       <c r="CL14" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="CM14" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="CN14" s="13" t="s">
         <v>73</v>
       </c>
       <c r="CO14" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="CP14" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="CQ14" s="13" t="s">
         <v>7</v>
       </c>
       <c r="CR14" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="CS14" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="CT14" s="12"/>
       <c r="CU14" s="12"/>
@@ -10127,7 +10153,7 @@
         <v>67</v>
       </c>
       <c r="CX14" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="CY14" s="13" t="s">
         <v>67</v>
@@ -10142,10 +10168,10 @@
         <v>74</v>
       </c>
       <c r="DG14" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="DH14" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="DI14" s="12"/>
       <c r="DJ14" s="12"/>
@@ -10154,28 +10180,28 @@
         <v>67</v>
       </c>
       <c r="DM14" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="DN14" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="DO14" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="DP14" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="DQ14" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="DR14" s="13" t="s">
         <v>16</v>
       </c>
       <c r="DS14" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="DT14" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="DU14" s="12"/>
       <c r="DV14" s="12"/>
@@ -10196,85 +10222,85 @@
         <v>67</v>
       </c>
       <c r="EK14" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="EL14" s="27" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:142">
       <c r="A15" s="1"/>
       <c r="B15" s="20" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="C15" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="D15" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="E15" s="13" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="F15" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="G15" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="H15" s="13" t="s">
         <v>210</v>
       </c>
       <c r="I15" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="J15" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="K15" s="13" t="s">
         <v>220</v>
       </c>
       <c r="L15" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="M15" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="N15" s="13" t="s">
         <v>209</v>
       </c>
       <c r="O15" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="P15" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="Q15" s="13" t="s">
         <v>160</v>
       </c>
       <c r="R15" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="S15" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="T15" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="U15" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="V15" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="W15" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="X15" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="Y15" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="Z15" s="12"/>
       <c r="AA15" s="12"/>
@@ -10304,19 +10330,19 @@
         <v>91</v>
       </c>
       <c r="AY15" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="AZ15" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="BA15" s="13" t="s">
         <v>160</v>
       </c>
       <c r="BB15" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="BC15" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="BD15" s="12"/>
       <c r="BE15" s="12"/>
@@ -10334,13 +10360,13 @@
         <v>16</v>
       </c>
       <c r="BQ15" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="BR15" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="BS15" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="BT15" s="13" t="s">
         <v>160</v>
@@ -10352,37 +10378,37 @@
         <v>173</v>
       </c>
       <c r="BW15" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="BX15" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="BY15" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="BZ15" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="CA15" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="CB15" s="13" t="s">
         <v>194</v>
       </c>
       <c r="CC15" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="CD15" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="CE15" s="13" t="s">
         <v>73</v>
       </c>
       <c r="CF15" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="CG15" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="CH15" s="12"/>
       <c r="CI15" s="12"/>
@@ -10400,136 +10426,136 @@
         <v>16</v>
       </c>
       <c r="CU15" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="CV15" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="CW15" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="CX15" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="CY15" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="CZ15" s="13" t="s">
         <v>73</v>
       </c>
       <c r="DA15" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="DB15" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="DC15" s="13" t="s">
         <v>73</v>
       </c>
       <c r="DD15" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="DE15" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="DF15" s="13" t="s">
         <v>16</v>
       </c>
       <c r="DG15" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="DH15" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="DI15" s="13" t="s">
         <v>62</v>
       </c>
       <c r="DJ15" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="DK15" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="DL15" s="13" t="s">
         <v>16</v>
       </c>
       <c r="DM15" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="DN15" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="DO15" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="DP15" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="DQ15" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="DR15" s="13" t="s">
         <v>91</v>
       </c>
       <c r="DS15" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="DT15" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="DU15" s="13" t="s">
         <v>91</v>
       </c>
       <c r="DV15" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="DW15" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="DX15" s="13" t="s">
         <v>194</v>
       </c>
       <c r="DY15" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="DZ15" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="EA15" s="13" t="s">
         <v>173</v>
       </c>
       <c r="EB15" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="EC15" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="ED15" s="13" t="s">
         <v>159</v>
       </c>
       <c r="EE15" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="EF15" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="EG15" s="13" t="s">
         <v>160</v>
       </c>
       <c r="EH15" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="EI15" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="EJ15" s="13" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="EK15" s="23" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="EL15" s="27" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:142">
@@ -10601,40 +10627,40 @@
       <c r="BN16" s="17"/>
       <c r="BO16" s="17"/>
       <c r="BP16" s="16" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="BQ16" s="24" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="BR16" s="24" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="BS16" s="24" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="BT16" s="24" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="BU16" s="24" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="BV16" s="16" t="s">
         <v>159</v>
       </c>
       <c r="BW16" s="24" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="BX16" s="24" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="BY16" s="24" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="BZ16" s="24" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="CA16" s="24" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="CB16" s="17"/>
       <c r="CC16" s="17"/>
@@ -10643,10 +10669,10 @@
         <v>173</v>
       </c>
       <c r="CF16" s="24" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="CG16" s="24" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="CH16" s="17"/>
       <c r="CI16" s="17"/>
@@ -10664,73 +10690,73 @@
         <v>91</v>
       </c>
       <c r="CU16" s="24" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="CV16" s="24" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="CW16" s="24" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="CX16" s="24" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="CY16" s="24" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="CZ16" s="16" t="s">
         <v>194</v>
       </c>
       <c r="DA16" s="24" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="DB16" s="24" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="DC16" s="16" t="s">
         <v>173</v>
       </c>
       <c r="DD16" s="24" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="DE16" s="24" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="DF16" s="16" t="s">
         <v>91</v>
       </c>
       <c r="DG16" s="24" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="DH16" s="24" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="DI16" s="16" t="s">
         <v>7</v>
       </c>
       <c r="DJ16" s="24" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="DK16" s="24" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="DL16" s="16" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="DM16" s="24" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="DN16" s="24" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="DO16" s="24" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="DP16" s="24" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="DQ16" s="24" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="DR16" s="17"/>
       <c r="DS16" s="17"/>
@@ -11188,5 +11214,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>